<commit_message>
Clean up code fix emission factors
</commit_message>
<xml_diff>
--- a/src/data/emission_factors.xlsx
+++ b/src/data/emission_factors.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahmoudmobir/Desktop/Work/zeolites/zeolites/app/services/calculate_emissions/shipping/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahmoudmobir/Desktop/Work/carbon_emissions/calculate_shipping_emissions/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A115F2-199A-E347-B79F-2266EEA363E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F4D0B4-4B75-1545-B25E-BBD2DC332434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15420" windowHeight="18900" activeTab="1" xr2:uid="{22EC22EC-EC97-5D42-B2C2-2A0AA22BFA4B}"/>
+    <workbookView xWindow="10540" yWindow="29560" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{22EC22EC-EC97-5D42-B2C2-2A0AA22BFA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="electricity_intensity" sheetId="10" r:id="rId1"/>
     <sheet name="emission_factors" sheetId="12" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">emission_factors!$A$1:$H$355</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,39 +55,6 @@
       </text>
     </comment>
     <comment ref="H41" authorId="1" shapeId="0" xr:uid="{9BDC6C5D-5568-F647-B28E-889368EFA0A4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mahmoud Mobir:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>g or kg?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I87" authorId="1" shapeId="0" xr:uid="{C07FAF1D-8EAA-0045-8A34-84ACA6DF39D1}">
       <text>
         <r>
           <rPr>
@@ -5516,10 +5486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAD11CE-5A50-1645-9349-499BE8283002}">
-  <dimension ref="A1:K368"/>
+  <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E280" workbookViewId="0">
-      <selection activeCell="G289" sqref="G289"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6903,7 +6873,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>434</v>
       </c>
@@ -6920,7 +6890,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>434</v>
       </c>
@@ -6937,7 +6907,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>434</v>
       </c>
@@ -6954,7 +6924,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -6971,7 +6941,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>434</v>
       </c>
@@ -6985,14 +6955,10 @@
         <v>501</v>
       </c>
       <c r="H85">
-        <f>I85*1.15</f>
         <v>919.99999999999989</v>
       </c>
-      <c r="I85" s="9">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>434</v>
       </c>
@@ -7006,14 +6972,10 @@
         <v>501</v>
       </c>
       <c r="H86">
-        <f t="shared" ref="H86:H89" si="0">I86*1.15</f>
         <v>362.25</v>
       </c>
-      <c r="I86" s="9">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>434</v>
       </c>
@@ -7027,14 +6989,10 @@
         <v>501</v>
       </c>
       <c r="H87">
-        <f t="shared" si="0"/>
         <v>224.24999999999997</v>
       </c>
-      <c r="I87" s="9">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>434</v>
       </c>
@@ -7048,14 +7006,10 @@
         <v>501</v>
       </c>
       <c r="H88">
-        <f t="shared" si="0"/>
         <v>132.25</v>
       </c>
-      <c r="I88" s="9">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>434</v>
       </c>
@@ -7069,14 +7023,10 @@
         <v>501</v>
       </c>
       <c r="H89">
-        <f>I89*1.12</f>
         <v>352.8</v>
       </c>
-      <c r="I89">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>434</v>
       </c>
@@ -7090,14 +7040,10 @@
         <v>501</v>
       </c>
       <c r="H90">
-        <f t="shared" ref="H90:H130" si="1">I90*1.12</f>
         <v>235.20000000000002</v>
       </c>
-      <c r="I90">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>434</v>
       </c>
@@ -7111,14 +7057,10 @@
         <v>501</v>
       </c>
       <c r="H91">
-        <f t="shared" si="1"/>
         <v>200.48000000000002</v>
       </c>
-      <c r="I91">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>434</v>
       </c>
@@ -7132,14 +7074,10 @@
         <v>501</v>
       </c>
       <c r="H92">
-        <f t="shared" si="1"/>
         <v>161.28000000000003</v>
       </c>
-      <c r="I92">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>434</v>
       </c>
@@ -7153,14 +7091,10 @@
         <v>501</v>
       </c>
       <c r="H93">
-        <f t="shared" si="1"/>
         <v>131.04000000000002</v>
       </c>
-      <c r="I93">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>434</v>
       </c>
@@ -7174,14 +7108,10 @@
         <v>501</v>
       </c>
       <c r="H94">
-        <f t="shared" si="1"/>
         <v>129.92000000000002</v>
       </c>
-      <c r="I94">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>434</v>
       </c>
@@ -7195,14 +7125,10 @@
         <v>501</v>
       </c>
       <c r="H95">
-        <f t="shared" si="1"/>
         <v>106.4</v>
       </c>
-      <c r="I95">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>434</v>
       </c>
@@ -7216,14 +7142,10 @@
         <v>501</v>
       </c>
       <c r="H96">
-        <f t="shared" si="1"/>
         <v>150.08000000000001</v>
       </c>
-      <c r="I96">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>434</v>
       </c>
@@ -7237,14 +7159,10 @@
         <v>501</v>
       </c>
       <c r="H97">
-        <f t="shared" si="1"/>
         <v>73.92</v>
       </c>
-      <c r="I97">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>434</v>
       </c>
@@ -7258,14 +7176,10 @@
         <v>501</v>
       </c>
       <c r="H98">
-        <f t="shared" si="1"/>
         <v>60.480000000000004</v>
       </c>
-      <c r="I98">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>434</v>
       </c>
@@ -7279,14 +7193,10 @@
         <v>501</v>
       </c>
       <c r="H99">
-        <f t="shared" si="1"/>
         <v>1074.0800000000002</v>
       </c>
-      <c r="I99">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>434</v>
       </c>
@@ -7300,14 +7210,10 @@
         <v>501</v>
       </c>
       <c r="H100">
-        <f t="shared" si="1"/>
         <v>967.68000000000006</v>
       </c>
-      <c r="I100">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>434</v>
       </c>
@@ -7321,14 +7227,10 @@
         <v>501</v>
       </c>
       <c r="H101">
-        <f t="shared" si="1"/>
         <v>1024.8000000000002</v>
       </c>
-      <c r="I101">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>434</v>
       </c>
@@ -7342,14 +7244,10 @@
         <v>501</v>
       </c>
       <c r="H102">
-        <f t="shared" si="1"/>
         <v>347.20000000000005</v>
       </c>
-      <c r="I102">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>434</v>
       </c>
@@ -7363,14 +7261,10 @@
         <v>501</v>
       </c>
       <c r="H103">
-        <f t="shared" si="1"/>
         <v>231.84000000000003</v>
       </c>
-      <c r="I103">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>434</v>
       </c>
@@ -7384,14 +7278,10 @@
         <v>501</v>
       </c>
       <c r="H104">
-        <f t="shared" si="1"/>
         <v>198.24</v>
       </c>
-      <c r="I104">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>434</v>
       </c>
@@ -7405,14 +7295,10 @@
         <v>501</v>
       </c>
       <c r="H105">
-        <f t="shared" si="1"/>
         <v>148.96</v>
       </c>
-      <c r="I105">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>434</v>
       </c>
@@ -7426,14 +7312,10 @@
         <v>501</v>
       </c>
       <c r="H106">
-        <f t="shared" si="1"/>
         <v>161.28000000000003</v>
       </c>
-      <c r="I106">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>434</v>
       </c>
@@ -7447,14 +7329,10 @@
         <v>501</v>
       </c>
       <c r="H107">
-        <f t="shared" si="1"/>
         <v>150.08000000000001</v>
       </c>
-      <c r="I107">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>434</v>
       </c>
@@ -7468,14 +7346,10 @@
         <v>501</v>
       </c>
       <c r="H108">
-        <f t="shared" si="1"/>
         <v>80.640000000000015</v>
       </c>
-      <c r="I108">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>434</v>
       </c>
@@ -7489,14 +7363,10 @@
         <v>501</v>
       </c>
       <c r="H109">
-        <f t="shared" si="1"/>
         <v>94.080000000000013</v>
       </c>
-      <c r="I109">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>434</v>
       </c>
@@ -7510,14 +7380,10 @@
         <v>501</v>
       </c>
       <c r="H110">
-        <f t="shared" si="1"/>
         <v>62.720000000000006</v>
       </c>
-      <c r="I110">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>434</v>
       </c>
@@ -7531,14 +7397,10 @@
         <v>501</v>
       </c>
       <c r="H111">
-        <f t="shared" si="1"/>
         <v>73.92</v>
       </c>
-      <c r="I111">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>434</v>
       </c>
@@ -7552,14 +7414,10 @@
         <v>501</v>
       </c>
       <c r="H112">
-        <f t="shared" si="1"/>
         <v>51.52</v>
       </c>
-      <c r="I112">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>434</v>
       </c>
@@ -7573,14 +7431,10 @@
         <v>501</v>
       </c>
       <c r="H113">
-        <f t="shared" si="1"/>
         <v>60.480000000000004</v>
       </c>
-      <c r="I113">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>434</v>
       </c>
@@ -7594,14 +7448,10 @@
         <v>501</v>
       </c>
       <c r="H114">
-        <f t="shared" si="1"/>
         <v>107.52000000000001</v>
       </c>
-      <c r="I114">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>434</v>
       </c>
@@ -7615,14 +7465,10 @@
         <v>501</v>
       </c>
       <c r="H115">
-        <f t="shared" si="1"/>
         <v>98.56</v>
       </c>
-      <c r="I115">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>434</v>
       </c>
@@ -7636,14 +7482,10 @@
         <v>501</v>
       </c>
       <c r="H116">
-        <f t="shared" si="1"/>
         <v>40.320000000000007</v>
       </c>
-      <c r="I116">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>434</v>
       </c>
@@ -7657,14 +7499,10 @@
         <v>501</v>
       </c>
       <c r="H117">
-        <f t="shared" si="1"/>
         <v>98.56</v>
       </c>
-      <c r="I117">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>434</v>
       </c>
@@ -7678,14 +7516,10 @@
         <v>501</v>
       </c>
       <c r="H118">
-        <f t="shared" si="1"/>
         <v>40.320000000000007</v>
       </c>
-      <c r="I118">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>434</v>
       </c>
@@ -7699,14 +7533,10 @@
         <v>501</v>
       </c>
       <c r="H119">
-        <f t="shared" si="1"/>
         <v>96.320000000000007</v>
       </c>
-      <c r="I119">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>434</v>
       </c>
@@ -7720,14 +7550,10 @@
         <v>501</v>
       </c>
       <c r="H120">
-        <f t="shared" si="1"/>
         <v>89.600000000000009</v>
       </c>
-      <c r="I120">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>434</v>
       </c>
@@ -7741,14 +7567,10 @@
         <v>501</v>
       </c>
       <c r="H121">
-        <f t="shared" si="1"/>
         <v>41.440000000000005</v>
       </c>
-      <c r="I121">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>434</v>
       </c>
@@ -7762,14 +7584,10 @@
         <v>502</v>
       </c>
       <c r="H122">
-        <f t="shared" si="1"/>
         <v>1.2320000000000002</v>
       </c>
-      <c r="I122">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>434</v>
       </c>
@@ -7783,14 +7601,10 @@
         <v>502</v>
       </c>
       <c r="H123">
-        <f t="shared" si="1"/>
         <v>0.57120000000000004</v>
       </c>
-      <c r="I123">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>434</v>
       </c>
@@ -7804,14 +7618,10 @@
         <v>502</v>
       </c>
       <c r="H124">
-        <f t="shared" si="1"/>
         <v>1.0080000000000002</v>
       </c>
-      <c r="I124">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>434</v>
       </c>
@@ -7825,14 +7635,10 @@
         <v>502</v>
       </c>
       <c r="H125">
-        <f t="shared" si="1"/>
         <v>0.43680000000000008</v>
       </c>
-      <c r="I125">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>434</v>
       </c>
@@ -7846,14 +7652,10 @@
         <v>502</v>
       </c>
       <c r="H126">
-        <f t="shared" si="1"/>
         <v>1.0080000000000002</v>
       </c>
-      <c r="I126">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>434</v>
       </c>
@@ -7867,14 +7669,10 @@
         <v>502</v>
       </c>
       <c r="H127">
-        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="I127">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>434</v>
       </c>
@@ -7888,14 +7686,10 @@
         <v>502</v>
       </c>
       <c r="H128">
-        <f t="shared" si="1"/>
         <v>0.50400000000000011</v>
       </c>
-      <c r="I128">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>434</v>
       </c>
@@ -7909,14 +7703,10 @@
         <v>502</v>
       </c>
       <c r="H129">
-        <f t="shared" si="1"/>
         <v>0.19040000000000004</v>
       </c>
-      <c r="I129">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>434</v>
       </c>
@@ -7930,14 +7720,10 @@
         <v>502</v>
       </c>
       <c r="H130">
-        <f t="shared" si="1"/>
         <v>0.35840000000000005</v>
       </c>
-      <c r="I130">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>434</v>
       </c>
@@ -7954,7 +7740,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>434</v>
       </c>
@@ -7971,7 +7757,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>434</v>
       </c>
@@ -7988,7 +7774,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>434</v>
       </c>
@@ -8005,7 +7791,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>434</v>
       </c>
@@ -8022,7 +7808,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>434</v>
       </c>
@@ -8039,7 +7825,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>434</v>
       </c>
@@ -8056,7 +7842,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>434</v>
       </c>
@@ -8073,7 +7859,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>434</v>
       </c>
@@ -8090,7 +7876,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>434</v>
       </c>
@@ -8107,7 +7893,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>434</v>
       </c>
@@ -8124,7 +7910,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>434</v>
       </c>
@@ -8141,7 +7927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>434</v>
       </c>
@@ -8158,7 +7944,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>434</v>
       </c>
@@ -8206,7 +7992,7 @@
         <v>501</v>
       </c>
       <c r="H146">
-        <v>0</v>
+        <v>1.359</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -8223,7 +8009,7 @@
         <v>501</v>
       </c>
       <c r="H147">
-        <v>0</v>
+        <v>1.2370000000000001</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -8240,7 +8026,7 @@
         <v>501</v>
       </c>
       <c r="H148">
-        <v>0</v>
+        <v>1.5089999999999999</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -8257,7 +8043,7 @@
         <v>501</v>
       </c>
       <c r="H149">
-        <v>0</v>
+        <v>0.81699999999999995</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -8274,7 +8060,7 @@
         <v>501</v>
       </c>
       <c r="H150">
-        <v>0</v>
+        <v>0.97099999999999997</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -8291,7 +8077,7 @@
         <v>501</v>
       </c>
       <c r="H151">
-        <v>0</v>
+        <v>0.629</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -10351,7 +10137,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>458</v>
       </c>
@@ -10368,7 +10154,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>458</v>
       </c>
@@ -10385,7 +10171,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>458</v>
       </c>
@@ -10402,7 +10188,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>458</v>
       </c>
@@ -10419,7 +10205,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>458</v>
       </c>
@@ -10436,7 +10222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>458</v>
       </c>
@@ -10453,7 +10239,7 @@
         <v>98.9</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>458</v>
       </c>
@@ -10470,7 +10256,7 @@
         <v>100.2</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>458</v>
       </c>
@@ -10487,7 +10273,7 @@
         <v>96.4</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>458</v>
       </c>
@@ -10504,7 +10290,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>458</v>
       </c>
@@ -10521,7 +10307,7 @@
         <v>47.8</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>458</v>
       </c>
@@ -10538,7 +10324,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>458</v>
       </c>
@@ -10555,7 +10341,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>458</v>
       </c>
@@ -10572,7 +10358,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>458</v>
       </c>
@@ -10589,7 +10375,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" s="8" t="s">
         <v>442</v>
       </c>
@@ -10609,9 +10395,9 @@
       <c r="H287" s="10">
         <v>0</v>
       </c>
-      <c r="K287" s="8"/>
-    </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J287" s="8"/>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" s="8" t="s">
         <v>442</v>
       </c>
@@ -10631,9 +10417,9 @@
       <c r="H288" s="10">
         <v>0</v>
       </c>
-      <c r="K288" s="8"/>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J288" s="8"/>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" s="8" t="s">
         <v>442</v>
       </c>
@@ -10653,9 +10439,9 @@
       <c r="H289" s="10">
         <v>0</v>
       </c>
-      <c r="K289" s="8"/>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J289" s="8"/>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" s="8" t="s">
         <v>442</v>
       </c>
@@ -10675,9 +10461,9 @@
       <c r="H290" s="10">
         <v>0</v>
       </c>
-      <c r="K290" s="8"/>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J290" s="8"/>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" s="8" t="s">
         <v>442</v>
       </c>
@@ -10697,9 +10483,9 @@
       <c r="H291" s="10">
         <v>0</v>
       </c>
-      <c r="K291" s="8"/>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J291" s="8"/>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" s="8" t="s">
         <v>442</v>
       </c>
@@ -10719,9 +10505,9 @@
       <c r="H292" s="10">
         <v>0</v>
       </c>
-      <c r="K292" s="8"/>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J292" s="8"/>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" s="8" t="s">
         <v>442</v>
       </c>
@@ -10741,9 +10527,9 @@
       <c r="H293" s="10">
         <v>0</v>
       </c>
-      <c r="K293" s="8"/>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J293" s="8"/>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" s="8" t="s">
         <v>442</v>
       </c>
@@ -10763,9 +10549,9 @@
       <c r="H294" s="10">
         <v>0</v>
       </c>
-      <c r="K294" s="8"/>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J294" s="8"/>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" s="8" t="s">
         <v>442</v>
       </c>
@@ -10785,9 +10571,9 @@
       <c r="H295" s="10">
         <v>0</v>
       </c>
-      <c r="K295" s="8"/>
-    </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J295" s="8"/>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" s="8" t="s">
         <v>442</v>
       </c>
@@ -10807,9 +10593,9 @@
       <c r="H296" s="10">
         <v>0</v>
       </c>
-      <c r="K296" s="8"/>
-    </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J296" s="8"/>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" s="8" t="s">
         <v>442</v>
       </c>
@@ -10829,9 +10615,9 @@
       <c r="H297" s="10">
         <v>0</v>
       </c>
-      <c r="K297" s="8"/>
-    </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J297" s="8"/>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" s="8" t="s">
         <v>442</v>
       </c>
@@ -10851,9 +10637,9 @@
       <c r="H298" s="10">
         <v>0</v>
       </c>
-      <c r="K298" s="8"/>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J298" s="8"/>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" s="8" t="s">
         <v>442</v>
       </c>
@@ -10873,9 +10659,9 @@
       <c r="H299" s="10">
         <v>0</v>
       </c>
-      <c r="K299" s="8"/>
-    </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J299" s="8"/>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" s="8" t="s">
         <v>442</v>
       </c>
@@ -10895,9 +10681,9 @@
       <c r="H300" s="10">
         <v>0</v>
       </c>
-      <c r="K300" s="8"/>
-    </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J300" s="8"/>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" s="8" t="s">
         <v>445</v>
       </c>
@@ -10920,7 +10706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" s="8" t="s">
         <v>445</v>
       </c>
@@ -10943,7 +10729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" s="8" t="s">
         <v>445</v>
       </c>
@@ -10966,7 +10752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" s="8" t="s">
         <v>445</v>
       </c>

</xml_diff>